<commit_message>
Finalizando gráficos para plages
</commit_message>
<xml_diff>
--- a/Exoplanets/55Cnc_e/55Cnce - Gráfico de D por T.xlsx
+++ b/Exoplanets/55Cnc_e/55Cnce - Gráfico de D por T.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\StarsAndExoplanets\Exoplanets\55Cnc_e\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\Exoplanets\55Cnc_e\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90E432C2-83A9-4768-9D91-27AB8D3EEE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9AAE40-4807-4782-AB46-3EA429A25A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{72DEB198-EF53-410F-9E28-B7CA56B1786E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{72DEB198-EF53-410F-9E28-B7CA56B1786E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,25 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>wav</t>
+  </si>
+  <si>
+    <t>Temp</t>
   </si>
 </sst>
 </file>
@@ -81,7 +73,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,15 +389,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF43BAB4-C2F9-400D-92B8-A835359DA679}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="P12" sqref="P12:T12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,8 +416,11 @@
       <c r="F1">
         <v>7172</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J1">
+        <v>5172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>417.7</v>
       </c>
@@ -445,7 +440,7 @@
         <v>283.22394203150748</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>452.1</v>
       </c>
@@ -464,8 +459,35 @@
       <c r="F3" s="1">
         <v>289.6882987073468</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>452.1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>521.5</v>
+      </c>
+      <c r="N3" s="1">
+        <v>563.5</v>
+      </c>
+      <c r="O3" s="1">
+        <v>614</v>
+      </c>
+      <c r="P3" s="1">
+        <v>664.6</v>
+      </c>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>486.8</v>
       </c>
@@ -484,8 +506,43 @@
       <c r="F4" s="1">
         <v>294.50413645759619</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <f>J4-100</f>
+        <v>1.9334880123743261</v>
+      </c>
+      <c r="J4">
+        <f>K4*100/5172</f>
+        <v>101.93348801237433</v>
+      </c>
+      <c r="K4">
+        <v>5272</v>
+      </c>
+      <c r="L4" s="1">
+        <v>375.69017542393726</v>
+      </c>
+      <c r="M4" s="1">
+        <v>363.35132060638654</v>
+      </c>
+      <c r="N4" s="1">
+        <v>357.75265758453133</v>
+      </c>
+      <c r="O4" s="1">
+        <v>352.45475500789161</v>
+      </c>
+      <c r="P4" s="1">
+        <v>347.19488560286391</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>521.5</v>
       </c>
@@ -504,8 +561,43 @@
       <c r="F5" s="1">
         <v>297.23763878608531</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <f t="shared" ref="I5:I8" si="0">J5-100</f>
+        <v>5.8004640371229641</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J8" si="1">K5*100/5172</f>
+        <v>105.80046403712296</v>
+      </c>
+      <c r="K5">
+        <v>5472</v>
+      </c>
+      <c r="L5" s="1">
+        <v>368.90724514904161</v>
+      </c>
+      <c r="M5" s="1">
+        <v>357.84500566993228</v>
+      </c>
+      <c r="N5" s="1">
+        <v>352.79719981173849</v>
+      </c>
+      <c r="O5" s="1">
+        <v>348.03170535124826</v>
+      </c>
+      <c r="P5" s="1">
+        <v>343.21001157433528</v>
+      </c>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>556</v>
       </c>
@@ -524,8 +616,43 @@
       <c r="F6" s="1">
         <v>299.65938292420003</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>9.6674400618716163</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>109.66744006187162</v>
+      </c>
+      <c r="K6">
+        <v>5672</v>
+      </c>
+      <c r="L6" s="1">
+        <v>361.39575297344794</v>
+      </c>
+      <c r="M6" s="1">
+        <v>351.87075718656757</v>
+      </c>
+      <c r="N6" s="1">
+        <v>347.47377683108647</v>
+      </c>
+      <c r="O6" s="1">
+        <v>343.32735153219664</v>
+      </c>
+      <c r="P6" s="1">
+        <v>339.00668909880858</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>563.5</v>
       </c>
@@ -544,8 +671,43 @@
       <c r="F7" s="1">
         <v>299.90134729795949</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>19.334880123743233</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>119.33488012374323</v>
+      </c>
+      <c r="K7">
+        <v>6172</v>
+      </c>
+      <c r="L7" s="1">
+        <v>339.85551396442656</v>
+      </c>
+      <c r="M7" s="1">
+        <v>335.19102897627829</v>
+      </c>
+      <c r="N7" s="1">
+        <v>332.80849857331151</v>
+      </c>
+      <c r="O7" s="1">
+        <v>330.54203562676855</v>
+      </c>
+      <c r="P7" s="1">
+        <v>327.71229081007823</v>
+      </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>588.40000000000009</v>
       </c>
@@ -564,8 +726,43 @@
       <c r="F8" s="1">
         <v>301.57925014540064</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>38.669760247486465</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>138.66976024748647</v>
+      </c>
+      <c r="K8">
+        <v>7172</v>
+      </c>
+      <c r="L8" s="1">
+        <v>289.6882987073468</v>
+      </c>
+      <c r="M8" s="1">
+        <v>297.23763878608531</v>
+      </c>
+      <c r="N8" s="1">
+        <v>299.90134729795949</v>
+      </c>
+      <c r="O8" s="1">
+        <v>302.28481398220094</v>
+      </c>
+      <c r="P8" s="1">
+        <v>303.08320393501731</v>
+      </c>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>614</v>
       </c>
@@ -585,7 +782,7 @@
         <v>302.28481398220094</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>639</v>
       </c>
@@ -605,7 +802,7 @@
         <v>302.95248160761014</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>664.6</v>
       </c>
@@ -625,7 +822,7 @@
         <v>303.08320393501731</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>689.5</v>
       </c>
@@ -644,8 +841,23 @@
       <c r="F12" s="1">
         <v>303.96558377498997</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P12" s="1">
+        <v>347.19488560286391</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>343.21001157433528</v>
+      </c>
+      <c r="R12" s="1">
+        <v>339.00668909880858</v>
+      </c>
+      <c r="S12" s="1">
+        <v>327.71229081007823</v>
+      </c>
+      <c r="T12" s="1">
+        <v>303.08320393501731</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>715</v>
       </c>
@@ -665,7 +877,7 @@
         <v>304.03673976231448</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>740</v>
       </c>
@@ -685,7 +897,7 @@
         <v>304.16197939941992</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>765</v>
       </c>
@@ -704,8 +916,26 @@
       <c r="F15" s="1">
         <v>304.2404392411546</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>1.9334880123743261</v>
+      </c>
+      <c r="N15">
+        <v>1.9334880123743261</v>
+      </c>
+      <c r="O15">
+        <v>5.8004640371229641</v>
+      </c>
+      <c r="P15">
+        <v>9.6674400618716163</v>
+      </c>
+      <c r="Q15">
+        <v>19.334880123743233</v>
+      </c>
+      <c r="R15">
+        <v>38.669760247486465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>790.5</v>
       </c>
@@ -724,8 +954,11 @@
       <c r="F16" s="1">
         <v>304.58123989651756</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>5.8004640371229641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>816</v>
       </c>
@@ -744,8 +977,11 @@
       <c r="F17" s="1">
         <v>304.6048183186212</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>9.6674400618716163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>841.30000000000007</v>
       </c>
@@ -764,8 +1000,11 @@
       <c r="F18" s="1">
         <v>304.28715038455232</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>19.334880123743233</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>866</v>
       </c>
@@ -784,8 +1023,11 @@
       <c r="F19" s="1">
         <v>303.93644997928072</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>38.669760247486465</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>891.59999999999991</v>
       </c>
@@ -805,7 +1047,7 @@
         <v>304.10966662264281</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>917</v>
       </c>
@@ -825,7 +1067,7 @@
         <v>304.33846413457923</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>942.4</v>
       </c>
@@ -845,7 +1087,7 @@
         <v>304.59191750109585</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>967.30000000000007</v>
       </c>
@@ -865,7 +1107,7 @@
         <v>304.57707927589172</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>992.7</v>
       </c>
@@ -885,7 +1127,7 @@
         <v>305.14663382052998</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1018</v>
       </c>
@@ -905,7 +1147,7 @@
         <v>305.04673002362813</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1060</v>
       </c>
@@ -925,7 +1167,7 @@
         <v>304.67972868808425</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1098</v>
       </c>
@@ -945,7 +1187,7 @@
         <v>304.74621722853533</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1138</v>
       </c>
@@ -965,7 +1207,7 @@
         <v>305.21396040994466</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1179</v>
       </c>
@@ -985,7 +1227,7 @@
         <v>305.24242950913384</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1222</v>
       </c>
@@ -1005,7 +1247,7 @@
         <v>305.42790069032486</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1266</v>
       </c>
@@ -1025,7 +1267,7 @@
         <v>305.40025933645245</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1312</v>
       </c>
@@ -1045,7 +1287,7 @@
         <v>305.51713902193802</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1358</v>
       </c>
@@ -1065,7 +1307,7 @@
         <v>305.36567163130803</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>1408</v>
       </c>
@@ -1085,7 +1327,7 @@
         <v>304.59932360626942</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1459</v>
       </c>
@@ -1105,7 +1347,7 @@
         <v>304.05115193088415</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1512</v>
       </c>
@@ -1125,7 +1367,7 @@
         <v>302.96162171983275</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1566</v>
       </c>
@@ -1145,7 +1387,7 @@
         <v>301.79078981451556</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1623</v>
       </c>
@@ -1165,7 +1407,7 @@
         <v>300.71409974963268</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1682</v>
       </c>
@@ -1185,7 +1427,7 @@
         <v>300.83674897452005</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1743</v>
       </c>
@@ -1207,5 +1449,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>